<commit_message>
Break legends for scatMat working, but legend disappears and count values are logged with ggplotly
</commit_message>
<xml_diff>
--- a/tblshoot/Compare1/compare3.xlsx
+++ b/tblshoot/Compare1/compare3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7480" yWindow="0" windowWidth="10560" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="9260" yWindow="0" windowWidth="10560" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>limma</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>edger2</t>
-  </si>
-  <si>
-    <t>Ven</t>
   </si>
 </sst>
 </file>
@@ -528,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1470,11 +1467,6 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="H32" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>